<commit_message>
Datentyp Decimal und Numeric implementiert und getestet
git-svn-id: svn://localhost/Transferprojekt@69 d8cf526a-ed47-ab48-8470-8a9acf7b5d78
</commit_message>
<xml_diff>
--- a/csv2siard/torque-xml-sql99.xlsx
+++ b/csv2siard/torque-xml-sql99.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>BIT</t>
   </si>
@@ -117,9 +117,6 @@
     <t>ctype_digit</t>
   </si>
   <si>
-    <t>Typenprüfung</t>
-  </si>
-  <si>
     <t>is_numeric</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>xml_encode</t>
   </si>
   <si>
-    <t>bin2hex</t>
-  </si>
-  <si>
     <t>to_bool</t>
   </si>
   <si>
@@ -178,6 +172,19 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Typenprüfung &amp;
+Konvertierung</t>
+  </si>
+  <si>
+    <t>base64-&gt;hex</t>
+  </si>
+  <si>
+    <t>bin-&gt;hex</t>
+  </si>
+  <si>
+    <t>bit-&gt;hex</t>
   </si>
 </sst>
 </file>
@@ -401,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -423,6 +430,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -720,7 +730,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B31"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -730,18 +740,18 @@
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="30.75" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
+      <c r="B1" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -749,10 +759,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>0</v>
@@ -766,7 +776,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -780,7 +790,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -794,7 +804,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -808,7 +818,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
@@ -819,10 +829,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -833,10 +843,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
@@ -847,10 +857,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
@@ -861,10 +871,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
@@ -875,13 +885,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -889,13 +899,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -903,13 +913,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -917,10 +927,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>12</v>
@@ -931,10 +941,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -945,10 +955,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>14</v>
@@ -959,13 +969,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -973,13 +983,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -987,13 +997,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1001,13 +1011,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1015,13 +1025,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1029,13 +1039,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1043,13 +1053,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1057,13 +1067,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1071,13 +1081,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1085,10 +1095,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>24</v>
@@ -1099,13 +1109,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1114,10 +1124,10 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1125,13 +1135,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1139,13 +1149,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1">
@@ -1153,10 +1163,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Handbuch mit den Erweiterungen von 1.6.2 ergänzt
git-svn-id: svn://localhost/Transferprojekt@72 d8cf526a-ed47-ab48-8470-8a9acf7b5d78
</commit_message>
<xml_diff>
--- a/csv2siard/torque-xml-sql99.xlsx
+++ b/csv2siard/torque-xml-sql99.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>BIT</t>
   </si>
@@ -185,6 +185,51 @@
   </si>
   <si>
     <t>bit-&gt;hex</t>
+  </si>
+  <si>
+    <t>2003-12-31T01:02:03</t>
+  </si>
+  <si>
+    <t>2003-12-31</t>
+  </si>
+  <si>
+    <t>01:02:03</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ABV</t>
+  </si>
+  <si>
+    <t>Victor jagt zwölf Boxkämpfer quer über den Sylter Deich</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>00011011</t>
+  </si>
+  <si>
+    <t>VGhpcyBpcyBhbiBlbmNvZGVkIHN0cmluZw==</t>
+  </si>
+  <si>
+    <t>R0lGODlhDAAKAJEAAP///3N1B1FRUQAAACwAAAAADAAKAAACGpSPB8ttDcELNE5Ac5ACVww+ESOOnLkkqlEAADs=</t>
+  </si>
+  <si>
+    <t>The quick brown fox jumps over the lazy dog</t>
+  </si>
+  <si>
+    <t>http://ch.php.net/manual/en/function.base64-decode.php</t>
+  </si>
+  <si>
+    <t>A B C</t>
+  </si>
+  <si>
+    <t>CSV Sample Daten</t>
   </si>
 </sst>
 </file>
@@ -392,9 +437,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -408,29 +451,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -727,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E31" sqref="A1:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -738,443 +801,528 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9">
+        <v>-232767</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9">
+        <v>-2147483647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2147483647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>345.6789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1234567891234560</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1.23456789123456E+22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1234567891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9">
+        <v>12345678.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D17" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="E17" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60.75" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:5" ht="75">
+      <c r="A27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C28" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="E28" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45">
+      <c r="A29" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
+      <c r="E29" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D30" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
+      <c r="E30" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A31" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D31" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>5</v>
+      <c r="E31" s="19" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E17" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>